<commit_message>
Excel DataTable scripts completed.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Excel.xlsx
+++ b/src/test/resources/testdata/Excel.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EclipseInstallation\java frameworks\CucumberFramework3\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9D6F74-8A53-4B51-966D-3C15FEECD517}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF68A64-BCE9-4957-81B4-B1BC1DAC66D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="504" windowWidth="19416" windowHeight="10416" xr2:uid="{CD3A54CB-C005-0E4A-932C-421D6A132F4C}"/>
   </bookViews>
   <sheets>
     <sheet name="customerInfo" sheetId="1" r:id="rId1"/>
-    <sheet name="quoteChevron" sheetId="2" r:id="rId2"/>
-    <sheet name="Staff" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>FirstName</t>
   </si>
@@ -71,9 +69,6 @@
     <t>EffectiveDate</t>
   </si>
   <si>
-    <t>02172023</t>
-  </si>
-  <si>
     <t>Florida</t>
   </si>
   <si>
@@ -135,6 +130,9 @@
   </si>
   <si>
     <t>33811</t>
+  </si>
+  <si>
+    <t>02202023</t>
   </si>
 </sst>
 </file>
@@ -509,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D793F7-630D-9741-BAE5-9B86014DDE1E}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
@@ -556,31 +554,31 @@
         <v>12</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.4">
@@ -600,37 +598,37 @@
         <v>33837</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N2" s="6">
         <v>2022</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.4">
@@ -644,43 +642,43 @@
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="H3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N3" s="6">
         <v>2022</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="21" x14ac:dyDescent="0.4">
@@ -759,219 +757,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0CC62A-99F6-E84B-8CDF-3B8105EE77B0}">
-  <dimension ref="A1:J12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.796875" customWidth="1"/>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.796875" customWidth="1"/>
-    <col min="6" max="6" width="18.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2">
-        <v>8133216598</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2">
-        <v>7542326598</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A893316-75ED-1C4D-98B6-285C034C8FF2}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
API Testing feature file and step definitions created,POM updated.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Excel.xlsx
+++ b/src/test/resources/testdata/Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EclipseInstallation\java frameworks\CucumberFramework3\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF68A64-BCE9-4957-81B4-B1BC1DAC66D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B38315-FAA4-4A7A-AD07-36E890A64246}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="504" windowWidth="19416" windowHeight="10416" xr2:uid="{CD3A54CB-C005-0E4A-932C-421D6A132F4C}"/>
   </bookViews>
@@ -132,7 +132,7 @@
     <t>33811</t>
   </si>
   <si>
-    <t>02202023</t>
+    <t>02212023</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
API Regression Suite Scripts completed. First commit company repo.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Excel.xlsx
+++ b/src/test/resources/testdata/Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EclipseInstallation\java frameworks\CucumberFramework3\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEFFBE4-75A5-408F-973D-1E2DDE3C0173}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71FC74F-D82D-401B-A9BE-091A9C406BC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="504" windowWidth="19416" windowHeight="10416" xr2:uid="{CD3A54CB-C005-0E4A-932C-421D6A132F4C}"/>
   </bookViews>
@@ -132,7 +132,7 @@
     <t>33811</t>
   </si>
   <si>
-    <t>02232023</t>
+    <t>02272023</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Vol Product Lines have been updated.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Excel.xlsx
+++ b/src/test/resources/testdata/Excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EclipseInstallation\java frameworks\CucumberFramework3\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYavas\git\AutomationCucumber2023\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71FC74F-D82D-401B-A9BE-091A9C406BC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721F316C-817A-4C59-8954-EAE5CA271932}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="504" windowWidth="19416" windowHeight="10416" xr2:uid="{CD3A54CB-C005-0E4A-932C-421D6A132F4C}"/>
   </bookViews>
@@ -132,7 +132,7 @@
     <t>33811</t>
   </si>
   <si>
-    <t>02272023</t>
+    <t>07152023</t>
   </si>
 </sst>
 </file>
@@ -507,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D793F7-630D-9741-BAE5-9B86014DDE1E}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
TOMHPD, TOMHO, Datatables updated(Ho3,Ho4,Ho6)
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Excel.xlsx
+++ b/src/test/resources/testdata/Excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20400"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYavas\git\AutomationCucumber2023\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721F316C-817A-4C59-8954-EAE5CA271932}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4C222D-421A-4CB4-A274-956620ABA2F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="504" windowWidth="19416" windowHeight="10416" xr2:uid="{CD3A54CB-C005-0E4A-932C-421D6A132F4C}"/>
   </bookViews>
@@ -132,7 +132,7 @@
     <t>33811</t>
   </si>
   <si>
-    <t>07152023</t>
+    <t>07302023</t>
   </si>
 </sst>
 </file>
@@ -507,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D793F7-630D-9741-BAE5-9B86014DDE1E}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>

</xml_diff>